<commit_message>
saving dataset as csv instead of pickle now, cause: deviation of data
</commit_message>
<xml_diff>
--- a/main/CICIDS2018/results/results.xlsx
+++ b/main/CICIDS2018/results/results.xlsx
@@ -456,13 +456,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -508,13 +508,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D13" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -524,13 +524,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D14" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -540,13 +540,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D15" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -597,13 +597,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -611,13 +611,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.213806539773941</v>
+        <v>0.01773619651794434</v>
       </c>
       <c r="C3" t="n">
-        <v>0.888093888759613</v>
+        <v>0.9948400259017944</v>
       </c>
       <c r="D3" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -663,13 +663,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.213806539773941</v>
+        <v>0.01773619651794434</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D13" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -679,13 +679,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C14" t="n">
-        <v>0.888093888759613</v>
+        <v>0.9948400259017944</v>
       </c>
       <c r="D14" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -695,13 +695,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4230037182569504</v>
+        <v>0.5048428475856781</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8758645951747894</v>
+        <v>0.9869800209999084</v>
       </c>
       <c r="D15" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -711,10 +711,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2958494870208568</v>
+        <v>0.6888728322621279</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01729483284589983</v>
+        <v>0.01111572553256617</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -761,13 +761,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -775,13 +775,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.213806539773941</v>
+        <v>0.01773619651794434</v>
       </c>
       <c r="C3" t="n">
-        <v>0.888093888759613</v>
+        <v>0.9948400259017944</v>
       </c>
       <c r="D3" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -789,13 +789,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.427804172039032</v>
+        <v>0.0266546867787838</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8823458552360535</v>
+        <v>0.9916239380836487</v>
       </c>
       <c r="D4" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -841,13 +841,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.213806539773941</v>
+        <v>0.01773619651794434</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8636353015899658</v>
+        <v>0.9791200160980225</v>
       </c>
       <c r="D13" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -857,13 +857,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6322008967399597</v>
+        <v>0.9919494986534119</v>
       </c>
       <c r="C14" t="n">
-        <v>0.888093888759613</v>
+        <v>0.9948400259017944</v>
       </c>
       <c r="D14" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -873,13 +873,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.4246038695176442</v>
+        <v>0.34544679398338</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8780250151952108</v>
+        <v>0.9885279933611552</v>
       </c>
       <c r="D15" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -889,10 +889,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2092155370363859</v>
+        <v>0.5599055234826524</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0127889743755205</v>
+        <v>0.008304717475701578</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>

</xml_diff>